<commit_message>
Corrigir e ajustar documentação conforme orientação do professor.
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Riscos.xlsx
+++ b/planejamento/DP_Lista_Riscos.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Riscos!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -159,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -280,7 +280,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -298,7 +298,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,23 +307,23 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -645,7 +645,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -687,7 +687,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -713,7 +713,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -732,48 +732,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" s="17" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -781,7 +781,7 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>42077</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -790,7 +790,7 @@
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="10">
@@ -799,11 +799,11 @@
       <c r="G3" s="15">
         <v>0.4</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <f>+F3*G3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -823,7 +823,7 @@
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="10">
@@ -832,11 +832,11 @@
       <c r="G4" s="15">
         <v>0.5</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <f>+F4*G4</f>
         <v>1.5</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -856,7 +856,7 @@
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="10">
@@ -865,10 +865,10 @@
       <c r="G5" s="15">
         <v>0.3</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="20">
         <v>0.9</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>17</v>
       </c>
       <c r="J5" s="3" t="s">

</xml_diff>

<commit_message>
Correções e alterações na lista de riscos conforme orientação do Professor.
Correções e alterações na lista de riscos conforme orientação do
Professor.
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Riscos.xlsx
+++ b/planejamento/DP_Lista_Riscos.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="9345"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="9345" tabRatio="321"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Riscos!$2:$2</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Magnitude</t>
   </si>
@@ -115,9 +116,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Prazo</t>
-  </si>
-  <si>
     <t xml:space="preserve"> D</t>
   </si>
   <si>
@@ -136,22 +134,94 @@
     <t>Adriano/Waltson</t>
   </si>
   <si>
-    <t>A Não aceitação do aplicativo no mercado.</t>
-  </si>
-  <si>
-    <t>Divulgar ao máximo o aplicativo e tentar demostrar os benefícios oferecidos com a sua utilização.</t>
-  </si>
-  <si>
-    <t>Corremos o risco de o usuário final não gosta do aplicaivo ou mesmo nem dar créditos.</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do aplicativo pode ser afetado com o não cumprimento dos prazos.</t>
-  </si>
-  <si>
-    <t>Monitorar o Envio e o desenvolvimento das tarefas, assim controlando os prazos estabelecidos.</t>
-  </si>
-  <si>
     <t>Aprofundar nossos conhecimentos em um um curto prazo de tempo (em media 3 semanas), desenvolvendo um projeto piloto, integrando com as API's do Google como tambem de redes sociais.</t>
+  </si>
+  <si>
+    <t>Procurar na internet e entrar em contato com a própria Google para facilitar o processo.</t>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Não ter recursos (hardware e software) sufucientes para o término do projeto a tempo.</t>
+  </si>
+  <si>
+    <t>Alocar os Recursos em tempo Hábil.</t>
+  </si>
+  <si>
+    <t>Conexão API Facebbok</t>
+  </si>
+  <si>
+    <t>Conexão API Google</t>
+  </si>
+  <si>
+    <t>Desistenca de algum Integrante da equipe</t>
+  </si>
+  <si>
+    <t>Algum colaborador poderar vir a desistir da cadeira e prejudicar o andamento do projeto.</t>
+  </si>
+  <si>
+    <t>Acompanhar e gerenciar de perto todas as tarefas desenvolvidas por toda equipe envolvida, para redistribuir as demandas e retomar as tarefas do ponto onde parou.</t>
+  </si>
+  <si>
+    <t>Imprevistos com a conexão na API de busca do Google.</t>
+  </si>
+  <si>
+    <t>Imprevistos com a conexão na API de autenticação do Facebook.</t>
+  </si>
+  <si>
+    <t>Risco de erro na plataforma</t>
+  </si>
+  <si>
+    <t>Pesquisar por meio de ferramentas online, a solução para o erro encontrado</t>
+  </si>
+  <si>
+    <t>Risco Arquitetural</t>
+  </si>
+  <si>
+    <t>Mudanças devem ser realizadas na arquitetura do sistema, para diminuir a probabilidade ou o impacto de ameaças à segurança.</t>
+  </si>
+  <si>
+    <t>Contratar empresa de locação de Gerador Elétrico e que será responsável também pela prestação de serviço de instalação e manutenção do mesmo.</t>
+  </si>
+  <si>
+    <t>Pode ser necessário realizarmos o conserto ou substituição de equipamentos que vierem a apresentar defeitos.</t>
+  </si>
+  <si>
+    <t>Contratar empresa de manutenção para os equipamentos elétrico/eletrônicos que serão utilizados por toda a equipe de desenvolvimento de software.</t>
+  </si>
+  <si>
+    <t>Sempre realizar atualizações dos documentos de forma rotineira e não deixar muitas atualizações pra um tempo curto.</t>
+  </si>
+  <si>
+    <t>Atualizações realizadas ao longo de toda a semana, preferencialmente todos os dias úteis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemas da falta de um ambiente local usado para testes da infra-estrutura </t>
+  </si>
+  <si>
+    <t>Realizar cópia atualizada a cada alteração no projeto e disponibilizar para testes em outros possiveis ambientes.</t>
+  </si>
+  <si>
+    <t>A plataforma pode está configurada mas não emula o projeto corretamente.</t>
+  </si>
+  <si>
+    <t>É possível que ocorram problemas diversos com o fornecimento de energia elétrica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interrupção no fornecimento de energia elétrica.</t>
+  </si>
+  <si>
+    <t>Queima de equipamentos utiilizados pela a equipe de desenvolvimento de software.</t>
+  </si>
+  <si>
+    <t>O projeto pode ter riscos de segurança, onde se o mesmo não for tratado, poderá impactar negativamente no projeto.</t>
+  </si>
+  <si>
+    <t>Risco de não terminar as atividades em tempo hábil para a entrega final do projeto.</t>
+  </si>
+  <si>
+    <t>Necessário a cópia do projeto para realização de testes fora do ambiente inicial.</t>
   </si>
 </sst>
 </file>
@@ -167,10 +237,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -178,12 +244,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -203,6 +263,18 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -258,78 +330,105 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -646,7 +745,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -688,7 +787,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -711,343 +810,457 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="78.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="3" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="112.140625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="130.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="173.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" ht="45">
+      <c r="A1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+    </row>
+    <row r="2" spans="1:10" s="12" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>42077</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6">
         <v>5</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="25.5">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19">
-        <v>42077</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="10">
-        <v>5</v>
-      </c>
-      <c r="G3" s="15">
+      <c r="G3" s="11">
         <v>0.4</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="15">
         <f>+F3*G3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:10" s="32" customFormat="1">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26">
+        <v>42079</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1">
-      <c r="A4" s="3">
+      <c r="D4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6">
+        <v>5</v>
+      </c>
+      <c r="G4" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="H4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>42077</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="I4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="32" customFormat="1">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26">
+        <v>42079</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="H5" s="16">
+        <v>4</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" s="5" customFormat="1">
+      <c r="A6" s="27">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26">
+        <v>42079</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="H6" s="16">
+        <v>4</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="11" t="s">
+    </row>
+    <row r="7" spans="1:10" s="5" customFormat="1">
+      <c r="A7" s="27">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26">
+        <v>42080</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="15">
+        <f>+F7*G7</f>
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="5" customFormat="1">
+      <c r="A8" s="27">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26">
+        <v>42080</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ref="H8:H12" si="0">+F8*G8</f>
+        <v>2</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="5" customFormat="1">
+      <c r="A9" s="27">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26">
+        <v>42080</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="10">
-        <v>3</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="20">
-        <f>+F4*G4</f>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="8" customFormat="1">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
-        <v>42079</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="I9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="27">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26">
+        <v>42082</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="25.5">
+      <c r="A11" s="27">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26">
+        <v>42083</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="27">
+        <v>10</v>
+      </c>
+      <c r="B12" s="26">
+        <v>42087</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5">
+      <c r="A13" s="27">
+        <v>11</v>
+      </c>
+      <c r="B13" s="26">
+        <v>42088</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="20">
+        <v>5</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="22">
+        <f t="shared" ref="H13" si="1">+F13*G13</f>
+        <v>1.25</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="27">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="27">
         <v>13</v>
       </c>
-      <c r="F5" s="10">
-        <v>3</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H5" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" s="8" customFormat="1">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="7">
-        <f t="shared" ref="H7:H11" si="0">+F7*G7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" s="8" customFormat="1">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" s="8" customFormat="1">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" s="8" customFormat="1">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" s="8" customFormat="1">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1061,4 +1274,18 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alinhando as entregas dos documentos de Arquitetura e Riscos.
Alinhando as entregas dos documentos de Arquitetura e Riscos.
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Riscos.xlsx
+++ b/planejamento/DP_Lista_Riscos.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Magnitude</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Lista de Riscos: DoadorPE\Projeto-de-Software\planejamento</t>
   </si>
   <si>
-    <t>Android Platform Developer</t>
-  </si>
-  <si>
     <t>Contato inicial com a linguagem, Conhecimento tácito muito básico, no momento não satisfatório para que a conclusão do projeto seja o almejado.</t>
   </si>
   <si>
@@ -137,91 +134,52 @@
     <t>Aprofundar nossos conhecimentos em um um curto prazo de tempo (em media 3 semanas), desenvolvendo um projeto piloto, integrando com as API's do Google como tambem de redes sociais.</t>
   </si>
   <si>
-    <t>Procurar na internet e entrar em contato com a própria Google para facilitar o processo.</t>
-  </si>
-  <si>
-    <t>Recursos</t>
-  </si>
-  <si>
-    <t>Não ter recursos (hardware e software) sufucientes para o término do projeto a tempo.</t>
-  </si>
-  <si>
-    <t>Alocar os Recursos em tempo Hábil.</t>
-  </si>
-  <si>
-    <t>Conexão API Facebbok</t>
-  </si>
-  <si>
-    <t>Conexão API Google</t>
-  </si>
-  <si>
-    <t>Desistenca de algum Integrante da equipe</t>
-  </si>
-  <si>
-    <t>Algum colaborador poderar vir a desistir da cadeira e prejudicar o andamento do projeto.</t>
-  </si>
-  <si>
     <t>Acompanhar e gerenciar de perto todas as tarefas desenvolvidas por toda equipe envolvida, para redistribuir as demandas e retomar as tarefas do ponto onde parou.</t>
   </si>
   <si>
-    <t>Imprevistos com a conexão na API de busca do Google.</t>
-  </si>
-  <si>
-    <t>Imprevistos com a conexão na API de autenticação do Facebook.</t>
-  </si>
-  <si>
-    <t>Risco de erro na plataforma</t>
-  </si>
-  <si>
     <t>Pesquisar por meio de ferramentas online, a solução para o erro encontrado</t>
   </si>
   <si>
-    <t>Risco Arquitetural</t>
-  </si>
-  <si>
     <t>Mudanças devem ser realizadas na arquitetura do sistema, para diminuir a probabilidade ou o impacto de ameaças à segurança.</t>
   </si>
   <si>
-    <t>Contratar empresa de locação de Gerador Elétrico e que será responsável também pela prestação de serviço de instalação e manutenção do mesmo.</t>
-  </si>
-  <si>
-    <t>Pode ser necessário realizarmos o conserto ou substituição de equipamentos que vierem a apresentar defeitos.</t>
-  </si>
-  <si>
-    <t>Contratar empresa de manutenção para os equipamentos elétrico/eletrônicos que serão utilizados por toda a equipe de desenvolvimento de software.</t>
-  </si>
-  <si>
-    <t>Sempre realizar atualizações dos documentos de forma rotineira e não deixar muitas atualizações pra um tempo curto.</t>
-  </si>
-  <si>
-    <t>Atualizações realizadas ao longo de toda a semana, preferencialmente todos os dias úteis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problemas da falta de um ambiente local usado para testes da infra-estrutura </t>
-  </si>
-  <si>
     <t>Realizar cópia atualizada a cada alteração no projeto e disponibilizar para testes em outros possiveis ambientes.</t>
   </si>
   <si>
-    <t>A plataforma pode está configurada mas não emula o projeto corretamente.</t>
-  </si>
-  <si>
-    <t>É possível que ocorram problemas diversos com o fornecimento de energia elétrica.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Interrupção no fornecimento de energia elétrica.</t>
-  </si>
-  <si>
-    <t>Queima de equipamentos utiilizados pela a equipe de desenvolvimento de software.</t>
-  </si>
-  <si>
-    <t>O projeto pode ter riscos de segurança, onde se o mesmo não for tratado, poderá impactar negativamente no projeto.</t>
-  </si>
-  <si>
-    <t>Risco de não terminar as atividades em tempo hábil para a entrega final do projeto.</t>
-  </si>
-  <si>
-    <t>Necessário a cópia do projeto para realização de testes fora do ambiente inicial.</t>
+    <t>Algum integrante da equipe poderar vir a desistir da cadeira e prejudicar o andamento do projeto.</t>
+  </si>
+  <si>
+    <t>O projeto pode ter riscos de segurança onde poderá impactar negativamente na entrega do projeto caso o mesmo não for tratado.</t>
+  </si>
+  <si>
+    <t>A plataforma pode está configurada mas não emula o projeto corretamente no momento proposto a apresentação do projeto.</t>
+  </si>
+  <si>
+    <t>Ambiente local para testes da infra-estrutura.</t>
+  </si>
+  <si>
+    <t>Problemas da falta de um ambiente local usado para testes da infra-estrutura onde será necessário a cópia do projeto para realização de testes fora do ambiente inicial.</t>
+  </si>
+  <si>
+    <t>Android Platform Developer.</t>
+  </si>
+  <si>
+    <t>Recursos.</t>
+  </si>
+  <si>
+    <t>Risco de erro na plataforma.</t>
+  </si>
+  <si>
+    <t>Segurança.</t>
+  </si>
+  <si>
+    <t>Não ter recursos (hardware e software) sufucientes para o término do projeto em tempo hábil.</t>
+  </si>
+  <si>
+    <t>Alocar os Recursos em tempo Hábil. (Adquirimos um novo Notebook)</t>
+  </si>
+  <si>
+    <t>Desistencia.</t>
   </si>
 </sst>
 </file>
@@ -231,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -263,12 +221,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -333,18 +285,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -360,12 +306,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -379,51 +319,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -432,6 +349,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -745,7 +667,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -787,7 +709,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -810,457 +732,325 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="130.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="151.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="173.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-    </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="73.5">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1">
-      <c r="A3" s="7">
+    <row r="3" spans="1:10" s="3" customFormat="1">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="18">
         <v>42077</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>5</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="6">
         <v>0.4</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="7">
         <f>+F3*G3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>42079</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H4" s="14">
+        <f>+F4*G4</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1">
+      <c r="A5" s="19">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18">
+        <v>42080</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="7">
+        <f>+F5*G5</f>
+        <v>2.5</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="32" customFormat="1">
-      <c r="A4" s="31">
+    <row r="6" spans="1:10" s="3" customFormat="1">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18">
+        <v>42097</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" ref="H6:H9" si="0">+F6*G6</f>
         <v>2</v>
       </c>
-      <c r="B4" s="26">
-        <v>42079</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="I6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1">
+      <c r="A7" s="19">
         <v>5</v>
       </c>
-      <c r="G4" s="17">
-        <v>0.25</v>
-      </c>
-      <c r="H4" s="16">
-        <v>2</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="32" customFormat="1">
-      <c r="A5" s="31">
-        <v>3</v>
-      </c>
-      <c r="B5" s="26">
-        <v>42079</v>
-      </c>
-      <c r="C5" s="28" t="s">
+      <c r="B7" s="18">
+        <v>42099</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="H5" s="16">
-        <v>4</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" s="5" customFormat="1">
-      <c r="A6" s="27">
-        <v>4</v>
-      </c>
-      <c r="B6" s="26">
-        <v>42079</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="17">
-        <v>0.15</v>
-      </c>
-      <c r="H6" s="16">
-        <v>4</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="5" customFormat="1">
-      <c r="A7" s="27">
+      <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="26">
-        <v>42080</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="15">
-        <f>+F7*G7</f>
-        <v>2.5</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="5" customFormat="1">
-      <c r="A8" s="27">
-        <v>6</v>
-      </c>
-      <c r="B8" s="26">
-        <v>42080</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" ref="H8:H12" si="0">+F8*G8</f>
-        <v>2</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="5" customFormat="1">
-      <c r="A9" s="27">
-        <v>7</v>
-      </c>
-      <c r="B9" s="26">
-        <v>42080</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="G7" s="6">
         <v>0.3</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="27">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26">
-        <v>42082</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="7">
-        <v>5</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="27">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26">
-        <v>42083</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="I7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18">
+        <v>42099</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="27">
-        <v>10</v>
-      </c>
-      <c r="B12" s="26">
-        <v>42087</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8">
+      <c r="G8" s="6">
         <v>0.2</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="27">
-        <v>11</v>
-      </c>
-      <c r="B13" s="26">
-        <v>42088</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="F13" s="20">
-        <v>5</v>
-      </c>
-      <c r="G13" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="H13" s="22">
-        <f t="shared" ref="H13" si="1">+F13*G13</f>
-        <v>1.25</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="27">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="27">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="23"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Ajustes na Lisda de Riscos, conforme orientação do Professor.
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Riscos.xlsx
+++ b/planejamento/DP_Lista_Riscos.xlsx
@@ -137,9 +137,6 @@
     <t>Acompanhar e gerenciar de perto todas as tarefas desenvolvidas por toda equipe envolvida, para redistribuir as demandas e retomar as tarefas do ponto onde parou.</t>
   </si>
   <si>
-    <t>Pesquisar por meio de ferramentas online, a solução para o erro encontrado</t>
-  </si>
-  <si>
     <t>Mudanças devem ser realizadas na arquitetura do sistema, para diminuir a probabilidade ou o impacto de ameaças à segurança.</t>
   </si>
   <si>
@@ -152,12 +149,6 @@
     <t>O projeto pode ter riscos de segurança onde poderá impactar negativamente na entrega do projeto caso o mesmo não for tratado.</t>
   </si>
   <si>
-    <t>A plataforma pode está configurada mas não emula o projeto corretamente no momento proposto a apresentação do projeto.</t>
-  </si>
-  <si>
-    <t>Ambiente local para testes da infra-estrutura.</t>
-  </si>
-  <si>
     <t>Problemas da falta de um ambiente local usado para testes da infra-estrutura onde será necessário a cópia do projeto para realização de testes fora do ambiente inicial.</t>
   </si>
   <si>
@@ -167,9 +158,6 @@
     <t>Recursos.</t>
   </si>
   <si>
-    <t>Risco de erro na plataforma.</t>
-  </si>
-  <si>
     <t>Segurança.</t>
   </si>
   <si>
@@ -180,6 +168,18 @@
   </si>
   <si>
     <t>Desistencia.</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Ambiente local para testes.</t>
+  </si>
+  <si>
+    <t>Apesar de usarmos uma ferramenta de gerencia de configuração de software e alguns artificios tecnologico na comunicação, o tempo parece ser nosso maior arquirival. Pois  estamos nos dividindo constantemente entre as muitas tarefas da faculdade, as atividades particular do projeto e a vida pessoal. e nossa geografia não ajuda nos contatos o quanto precisaria.</t>
+  </si>
+  <si>
+    <t>Aproveitar o tempo restante nos dias de aula da cadeira em questão para adiantar o projeto e tirar as muitas dúvidas com o professor e entre a equipe, que constantemente vam sugindo durante o avanço do projeto.</t>
   </si>
 </sst>
 </file>
@@ -229,7 +229,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,6 +348,30 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,7 +697,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -709,7 +739,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -734,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -806,7 +836,7 @@
         <v>42077</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -839,10 +869,10 @@
         <v>42079</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>12</v>
@@ -861,7 +891,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1">
@@ -872,10 +902,10 @@
         <v>42080</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -897,37 +927,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1">
-      <c r="A6" s="19">
+    <row r="6" spans="1:10" s="28" customFormat="1" ht="38.25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="21">
         <v>42097</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="24">
         <v>5</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="25">
         <v>0.4</v>
       </c>
-      <c r="H6" s="7">
-        <f t="shared" ref="H6:H9" si="0">+F6*G6</f>
+      <c r="H6" s="26">
+        <f t="shared" ref="H6:H8" si="0">+F6*G6</f>
         <v>2</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>18</v>
+      <c r="J6" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1">
@@ -938,10 +968,10 @@
         <v>42099</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>12</v>
@@ -960,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -971,10 +1001,10 @@
         <v>42099</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>12</v>
@@ -993,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">

</xml_diff>

<commit_message>
Removendo e reorganizando Lista de Riscos
Removendo e reorganizando Lista de Riscos
</commit_message>
<xml_diff>
--- a/planejamento/DP_Lista_Riscos.xlsx
+++ b/planejamento/DP_Lista_Riscos.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Magnitude</t>
   </si>
@@ -116,9 +116,6 @@
     <t>D</t>
   </si>
   <si>
-    <t xml:space="preserve"> D</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -137,30 +134,15 @@
     <t>Acompanhar e gerenciar de perto todas as tarefas desenvolvidas por toda equipe envolvida, para redistribuir as demandas e retomar as tarefas do ponto onde parou.</t>
   </si>
   <si>
-    <t>Mudanças devem ser realizadas na arquitetura do sistema, para diminuir a probabilidade ou o impacto de ameaças à segurança.</t>
-  </si>
-  <si>
-    <t>Realizar cópia atualizada a cada alteração no projeto e disponibilizar para testes em outros possiveis ambientes.</t>
-  </si>
-  <si>
     <t>Algum integrante da equipe poderar vir a desistir da cadeira e prejudicar o andamento do projeto.</t>
   </si>
   <si>
-    <t>O projeto pode ter riscos de segurança onde poderá impactar negativamente na entrega do projeto caso o mesmo não for tratado.</t>
-  </si>
-  <si>
-    <t>Problemas da falta de um ambiente local usado para testes da infra-estrutura onde será necessário a cópia do projeto para realização de testes fora do ambiente inicial.</t>
-  </si>
-  <si>
     <t>Android Platform Developer.</t>
   </si>
   <si>
     <t>Recursos.</t>
   </si>
   <si>
-    <t>Segurança.</t>
-  </si>
-  <si>
     <t>Não ter recursos (hardware e software) sufucientes para o término do projeto em tempo hábil.</t>
   </si>
   <si>
@@ -168,18 +150,6 @@
   </si>
   <si>
     <t>Desistencia.</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>Ambiente local para testes.</t>
-  </si>
-  <si>
-    <t>Apesar de usarmos uma ferramenta de gerencia de configuração de software e alguns artificios tecnologico na comunicação, o tempo parece ser nosso maior arquirival. Pois  estamos nos dividindo constantemente entre as muitas tarefas da faculdade, as atividades particular do projeto e a vida pessoal. e nossa geografia não ajuda nos contatos o quanto precisaria.</t>
-  </si>
-  <si>
-    <t>Aproveitar o tempo restante nos dias de aula da cadeira em questão para adiantar o projeto e tirar as muitas dúvidas com o professor e entre a equipe, que constantemente vam sugindo durante o avanço do projeto.</t>
   </si>
 </sst>
 </file>
@@ -229,7 +199,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,12 +215,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -348,30 +312,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,7 +637,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -739,7 +679,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -762,10 +702,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -784,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="45">
       <c r="A1" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -836,10 +776,10 @@
         <v>42077</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -855,10 +795,10 @@
         <v>2</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1">
@@ -869,13 +809,13 @@
         <v>42079</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
@@ -888,10 +828,10 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1">
@@ -902,10 +842,10 @@
         <v>42080</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -921,110 +861,53 @@
         <v>2.5</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="28" customFormat="1" ht="38.25">
-      <c r="A6" s="24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1">
+      <c r="A6" s="19">
         <v>4</v>
       </c>
-      <c r="B6" s="21">
-        <v>42097</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="24">
-        <v>5</v>
-      </c>
-      <c r="G6" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="H6" s="26">
-        <f t="shared" ref="H6:H8" si="0">+F6*G6</f>
-        <v>2</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1">
+      <c r="B6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="19">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
-        <v>42099</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H7" s="7">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>18</v>
-      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="19">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="18">
-        <v>42099</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="H8" s="7">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="5">
@@ -1067,20 +950,6 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="5">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>